<commit_message>
modify: add mean square error
</commit_message>
<xml_diff>
--- a/2020_01_32769/test/test.xlsx
+++ b/2020_01_32769/test/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2020-master\2020_01_32769\paper_20032501\old\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2020-master_old\2020_01_32769\paper_20032501\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -278,7 +278,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -298,6 +298,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -583,8 +586,8 @@
   <dimension ref="A1:M248"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -2263,7 +2266,10 @@
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="H57" s="1"/>
+      <c r="H57" s="7">
+        <f>SUMXMY2(H2:H56, I2:I56)/55</f>
+        <v>17.522632212265126</v>
+      </c>
       <c r="I57" s="1"/>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.45">
@@ -3032,7 +3038,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="H1:I1048576">
+  <conditionalFormatting sqref="H1:I56 H58:I1048576 I57">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -3064,7 +3070,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H1:I1048576</xm:sqref>
+          <xm:sqref>H1:I56 H58:I1048576 I57</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>